<commit_message>
update excel & update foutje in whatsapp analysis
</commit_message>
<xml_diff>
--- a/NHC_analysis.xlsx
+++ b/NHC_analysis.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linth\PycharmProjects\Scientific_Prog\GitHub\BlackStoriesAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAE4866-EE9D-4D9F-99AA-4199AA0F3250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0539E0F-30D9-4B92-9E8E-878C43E85F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Medium</t>
   </si>
@@ -106,6 +119,9 @@
     <t>[{'role': 'system', 'content': 'You have to solve a black stories riddle. I tell you a black story and you have to solve it by asking me questions.\n                                    You have to solve the riddle with as little questions as possible.\n                                    The riddle tells you the end of a story and you have to find out what lead to this end. \n                                    When I tell you the riddle, you have to try to solve the riddle by asking questions that I can only answer by yes, no or not relevant to the story. \n                                    You will use my answers to solve the riddle and find the story that lead to the end.\n                                    I tell you when you have solved the riddle, then you give me a summary of the story of the riddle.\n                                    Note that giving a summary to guess the answer is also counting as one question'}, {'role': 'user', 'content': 'a man and a woman are walking into a pub. they order the same drink from the bartender. one of them dies and the other one lives. '}, {'role': 'assistant', 'content': 'Did the drink contain poison?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the woman die?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did someone else at the pub harm the man?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the man have a pre-existing health condition?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the man consume anything else besides the drink before his death?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the drinks have different temperatures?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the man drink something else other than the drink he ordered at the pub?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': "Was there something in the man's glass before the drink was poured?"}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did they drink at different speeds?'}, {'role': 'user', 'content': 'yes'}, {'role': 'assistant', 'content': 'Did the man drink faster than the woman?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'So the man died because he drank slower than the woman, correct?'}, {'role': 'user', 'content': 'yes'}, {'role': 'assistant', 'content': 'The summary of the story is: A man and a woman walked into a pub and ordered the same drink. The woman drank her drink quickly, while the man sipped his slower. The drinks had a slowly dissolving poison that would only be deadly if ingested over a longer period of time. So, the man who took his time drinking, consumed more of the poison and thus died. The woman because she drank quickly, ingested less of the poison and survived.'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Was there something wrong or deadly with the last part of the drink that the man reached because he drank slower?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Was the drink they ordered an alcoholic beverage?'}, {'role': 'user', 'content': 'not relevant'}, {'role': 'assistant', 'content': 'Did the man die from some type of external event or trigger while they were in the pub?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Was there something deadly or toxic within the drinks that got neutralized over time?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the man choke on his drink?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Was there something harmful in the drink that naturally sank to the bottom over time?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the woman do something to her drink before consuming it?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the drink they had ordered originally contain something harmful?'}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the ice in their drinks have anything to do with the death?'}, {'role': 'user', 'content': 'yes'}, {'role': 'assistant', 'content': "Did the woman's ice melt before she consumed her drink?"}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': "Did the ice in the man's drink contain a harmful substance?"}, {'role': 'user', 'content': 'yes'}, {'role': 'assistant', 'content': "Did the harmful substance in the man's ice start affecting him only after the ice began to melt?"}, {'role': 'user', 'content': 'yes'}, {'role': 'assistant', 'content': "The summary of the story is: A man and a woman walked into a pub and ordered the same drink. Each of their drinks contained ice, however, the ice in the man's drink contained a harmful substance. Since the woman drank her drink quickly, the ice in her drink did not have time to melt and release the harmful substance. But the man, who drank his drink slower, gave time for the ice to melt, releasing the harmful substance into his drink and leading to his demise."}, {'role': 'user', 'content': 'no'}, {'role': 'assistant', 'content': 'Did the woman finish her drink before the ice in her glass have a chance to fully melt?'}, {'role': 'user', 'content': 'yes'}, {'role': 'assistant', 'content': 'The summary of the story is: A man and a woman walked into a pub and ordered the same drink, both containing ice cubes. The ice cubes in the drinks were poisoned. The woman drank her drink quickly, not giving the ice cubes enough time to fully melt and release the poison into her drink. The man, on the other hand, drank slowly, the ice cubes in his drink melted and the poison was released into the drink, which led to his death.\n'}]</t>
   </si>
   <si>
+    <t>['Linthe Van Rooij: You have to solve a black stories riddle. I tell you a black story and you have to solve it by asking me questions.', 'Linthe Van Rooij: Lola goes to a friend of hers and receives a pair of shoes because they did not fit her friend. It will mean her death that same evening.', 'Thijs : Is her death related to the shoes', 'Linthe Van Rooij: yes', 'Thijs : Are they regular shoes?', 'Linthe Van Rooij: yes', 'Thijs : Is her friend willingly giving the shoes?', 'Linthe Van Rooij: yes', 'Thijs : Does her friend know about the death when it is happening', 'Linthe Van Rooij: no', 'Thijs : Did she die naturally?', 'Linthe Van Rooij: no', 'Thijs : She was murdered?', 'Linthe Van Rooij: no', 'Thijs : Accident?', 'Linthe Van Rooij: yes', 'Thijs : Did she trip because of the shoes?', 'Linthe Van Rooij: no', 'Thijs : Did sure have the shoes on when she died?', 'Linthe Van Rooij: yes', 'Thijs : Was there anything off about the shoes?', 'Linthe Van Rooij: no', 'Thijs : Was there anyone else involved in her death', 'Linthe Van Rooij: yes', 'Thijs : Did that person want the shoes', 'Linthe Van Rooij: no', 'Thijs : Did they make the accident happen', 'Linthe Van Rooij: yes', 'Thijs : Was the accident at home', 'Linthe Van Rooij: yes', 'Thijs : Was it her husband?', 'Linthe Van Rooij: yes', 'Thijs : Was her husband having an affair with the friend', 'Linthe Van Rooij: no', 'Thijs : Did she die because of air restriction? E.g. choked', 'Linthe Van Rooij: no', 'Linthe Van Rooij: What where they doing together?', "Thijs : We're they dancing?", 'Linthe Van Rooij: no', "Thijs : We're they moving", 'Linthe Van Rooij: false assumption they', 'Thijs : Was she moving', 'Linthe Van Rooij: no', 'Thijs : Was he moving', 'Linthe Van Rooij: yes', 'Thijs : Did he kill her by accident', 'Linthe Van Rooij: yes', 'Thijs : Did he trip over the shoes', 'Linthe Van Rooij: no', 'Thijs : Did he stab her', 'Linthe Van Rooij: no', 'Thijs : Was he taking a shower', 'Linthe Van Rooij: no', 'Thijs : Were they eating', 'Linthe Van Rooij: no', 'Thijs : Sleeping?', 'Linthe Van Rooij: no', 'Thijs : Cooking', 'Linthe Van Rooij: no', 'Thijs : Did he scare her', 'Linthe Van Rooij: no', 'Thijs : Hint', 'Linthe Van Rooij: ask about the hobbies of the man', 'Thijs : Was he a shoe maker', 'Linthe Van Rooij: no', 'Thijs : Did he have a workshop', 'Linthe Van Rooij: no', 'Thijs : Anything clothes, food or fashion related hobbies?', 'Linthe Van Rooij: no', 'Thijs : Anything with weapons?', 'Linthe Van Rooij: yes', 'Thijs : Swords?', 'Linthe Van Rooij: no', 'Thijs : Guns', 'Linthe Van Rooij: no', 'Thijs : Bow and arrow', 'Linthe Van Rooij: yes', 'Thijs : Did her shoes look like a target', 'Linthe Van Rooij: no', 'Thijs : Did he shoot her with an arrow', 'Linthe Van Rooij: yes', 'Linthe Van Rooij: what could have been different with other shoes', 'Thijs : Did he think she was an intruder', 'Linthe Van Rooij: no', 'Thijs : Did she have the same shoes as his targets', 'Linthe Van Rooij: no', 'Thijs : Was she taller because of the shoes', 'Linthe Van Rooij: yes', 'Thijs : Did he practice shooting stuff from her head but now she is taller thus he shot her in the head', 'Linthe Van Rooij: no', 'Thijs : Was she taller than a safety wall, so she could get hit', 'Linthe Van Rooij: no', 'Linthe Van Rooij: Could he see where he was aiming?', 'Thijs : Was he blind or blondfolded', 'Linthe Van Rooij: yes', 'Thijs : So he shoots arrows blind, and she hold up a target ðŸŽ¯, but because she is taller he missed and hit her', 'Linthe Van Rooij: ik keur hem goed!']</t>
+  </si>
+  <si>
     <t>{1: 'Was there a conflict or argument between the man and the woman?', 2: 'Did one of them use the pistol during their time at the table?', 3: 'Is the pistol relevant to the story?', 4: 'Is the game of checkers relevant to the story?', 5: 'Was the result of the checker game influencing what would happen with the pistol?', 6: 'Did they play checkers for their survival?', 7: 'Did the loser of the checker game have to use the pistol on themselves?', 8: 'Did the winner of the checker game have to use the pistol?', 9: 'Was the pistol a stake in the checker game?', 10: 'So, the story is about a man and a woman who decided to play a game of checkers. The pistol on the table was the stake for the game. The winner would get the pistol, but we don\'t know why they wanted it or what they intended to do with it. No one used the pistol during their time at the table.', 11: 'Was the pistol theirs to begin with? Not relevant for the story.', 12: 'Did the man win the checker game? Not relevant for the story.', 13: 'Did they have a plan to use the pistol after the game?', 14: 'Was the pistol meant to be used on someone else not present at the checker game?', 15: 'Were they playing the game to kill time, with an imminent threat lurking, and that\'s why the pistol was placed on the table between them?', 16: 'Did they intend to use the pistol as protection?', 17: 'Did they intend to use the pistol in a celebratory way, like firing it into the air, after the game?', 18: 'Did the intention to use the pistol depended on whether they won or lost the game of checkers?', 19: 'Did they intend to use the pistol to decide something or someone\'s fate?', 20: 'Did the winner of the checkers game get to decide the fate of a third party using the pistol?', 21: 'Did they intend to scare someone with the pistol after the game?', 22: 'Did the game of checkers help them to decide who should use the pistol?', 23: 'Did they play the game of checkers to decide who would be the one to use the pistol to decide the fate of the other person?', 24: 'Did they play the game of checkers to decide who gets to decide their own fate with the pistol?', 25: 'The story is about a man and a woman who are in a desperate situation. They are seated at a table playing a game of checkers, not due to a conflict or a playful challenge. The pistol on the table is a reminder of their bleak situation. The checkers game is not for mere entertainment; the stake is much higher. The winner of the game earns the right to decide their own fate using the pistol. The outcome of the game will decide who gets to use the pistol to make a significant decision about their own life.', 26: 'Is the situation life-threatening?', 27: 'Are they trapped or held hostage in a place from which they are unable to escape?', 28: 'The story revolves around a man and a woman who are trapped or held hostage in a place from which there\'s no escape. Facing a life-threatening situation, they decide to play a game of checkers, with a daunting stake - a pistol placed on the table. They are not playing out of leisure or conflict, but desperation. The winner of the game gets the right to decide their fate with the pistol. Rather than being at the mercy of their captors, they choose this way to have some control over their own lives.', 29: 'Are they trapped in an uninhabited or desolate location with no hope of rescue?', 30: 'Does the winner of the game intend to use the pistol to end his/her own life, to avoid a possibly worse fate?', 31: 'The story is about a man and woman who found themselves trapped in a desolate location with no hope of rescue. They faced dire circumstances and to avoid a possibly worse fate, they decided to play a game of checkers—the stake, however, was not traditional. A pistol was placed on the table, awaiting the game\'s outcome. Through this game, they seized what little control was left in their desperate situation. The winner won the morbid prize—the chance to use the pistol to end their own life, thus escaping the bleak reality before them.', 32: 'Are they trapped at sea on a vessel with no hope of being found?', 33: 'Are they trapped in a cold, desolate place like the Arctic or Antarctic regions?', 34: 'Are they trapped in a desert with no hope for rescue and no way of getting food or water?', 35: 'Are they trapped in a cave or underground with no way out?', 36: 'Are they stranded in space, like on a spaceship or a space station, with no hope of rescue?', 37: 'Are they trapped in a jungle or forest with no means of communication or ability to navigate their way out?', 38: 'Are they trapped in a post-apocalyptic setting without any survival resources?', 39: 'Are they trapped on a high mountain peak with harsh weather conditions and no possibility of rescue?', 40: 'Are they trapped in a war-torn region and the worse fate they fear is falling into the hands of enemy troops or insurgents?', 41: 'Are they trapped in a sinking ship or submerged submarine with no hope of rescue?', 42: 'Will the worse fate they fear be drowning or suffocating due to lack of oxygen in the sinking ship/submarine?', 43: 'Is the worse fate they\'re trying to avoid that of starvation or dehydration while being trapped in the ship/submarine?', 44: 'Did they choose to play a game of checkers to decide who would use the pistol to avoid the slow and painful death of dehydration?', 45: 'The story is about a man and woman, trapped in a submerged submarine with no chance of rescue, faced the grim reality of eventual dehydration. In an attempt to take control of their fate, they decided to play a game of checkers, with a unique stake: a pistol with a single bullet. The outcome of the game would determine who gets to use the pistol, offering a quick escape from their dire situation. The checkers game, thus, became a means for one of them to choose an immediate end over a slow and painful death.'}</t>
   </si>
   <si>
@@ -145,6 +161,9 @@
     <t>{1: 'Did the drink contain poison?', 2: 'Did the woman die?', 3: 'Did someone else at the pub harm the man?', 4: 'Did the man have a pre-existing health condition?', 5: 'Did the man consume anything else besides the drink before his death?', 6: 'Did the drinks have different temperatures?', 7: 'Did the man drink something else other than the drink he ordered at the pub?', 8: "Was there something in the man's glass before the drink was poured?", 9: 'Did they drink at different speeds?', 10: 'Did the man drink faster than the woman?', 11: 'So the man died because he drank slower than the woman, correct?', 12: 'The summary of the story is: A man and a woman walked into a pub and ordered the same drink. The woman drank her drink quickly, while the man sipped his slower. The drinks had a slowly dissolving poison that would only be deadly if ingested over a longer period of time. So, the man who took his time drinking, consumed more of the poison and thus died. The woman because she drank quickly, ingested less of the poison and survived.', 13: 'Was there something wrong or deadly with the last part of the drink that the man reached because he drank slower?', 14: 'Was the drink they ordered an alcoholic beverage?', 15: 'Did the man die from some type of external event or trigger while they were in the pub?', 16: 'Was there something deadly or toxic within the drinks that got neutralized over time?', 17: 'Did the man choke on his drink?', 18: 'Was there something harmful in the drink that naturally sank to the bottom over time?', 19: 'Did the woman do something to her drink before consuming it?', 20: 'Did the drink they had ordered originally contain something harmful?', 21: 'Did the ice in their drinks have anything to do with the death?', 22: "Did the woman's ice melt before she consumed her drink?", 23: "Did the ice in the man's drink contain a harmful substance?", 24: "Did the harmful substance in the man's ice start affecting him only after the ice began to melt?", 25: "The summary of the story is: A man and a woman walked into a pub and ordered the same drink. Each of their drinks contained ice, however, the ice in the man's drink contained a harmful substance. Since the woman drank her drink quickly, the ice in her drink did not have time to melt and release the harmful substance. But the man, who drank his drink slower, gave time for the ice to melt, releasing the harmful substance into his drink and leading to his demise.", 26: 'Did the woman finish her drink before the ice in her glass have a chance to fully melt?', 27: 'The summary of the story is: A man and a woman walked into a pub and ordered the same drink, both containing ice cubes. The ice cubes in the drinks were poisoned. The woman drank her drink quickly, not giving the ice cubes enough time to fully melt and release the poison into her drink. The man, on the other hand, drank slowly, the ice cubes in his drink melted and the poison was released into the drink, which led to his death.\n'}</t>
   </si>
   <si>
+    <t>['Is her death related to the shoes', 'Are they regular shoes?', 'Is her friend willingly giving the shoes?', 'Does her friend know about the death when it is happening', 'Did she die naturally?', 'She was murdered?', 'Accident?', 'Did she trip because of the shoes?', 'Did sure have the shoes on when she died?', 'Was there anything off about the shoes?', 'Was there anyone else involved in her death', 'Did that person want the shoes', 'Did they make the accident happen', 'Was the accident at home', 'Was it her husband?', 'Was her husband having an affair with the friend', 'Did she die because of air restriction? E.g. choked', "We're they dancing?", "We're they moving", 'Was she moving', 'Was he moving', 'Did he kill her by accident', 'Did he trip over the shoes', 'Did he stab her', 'Was he taking a shower', 'Were they eating', 'Sleeping?', 'Cooking', 'Did he scare her', 'Hint', 'Was he a shoe maker', 'Did he have a workshop', 'Anything clothes, food or fashion related hobbies?', 'Anything with weapons?', 'Swords?', 'Guns', 'Bow and arrow', 'Did her shoes look like a target', 'Did he shoot her with an arrow', 'Did he think she was an intruder', 'Did she have the same shoes as his targets', 'Was she taller because of the shoes', 'Did he practice shooting stuff from her head but now she is taller thus he shot her in the head', 'Was she taller than a safety wall, so she could get hit', 'Was he blind or blondfolded', 'So he shoots arrows blind, and she hold up a target ðŸŽ¯, but because she is taller he missed and hit her']</t>
+  </si>
+  <si>
     <t>['A man and a woman are seated at a table. On the table between them is a game of checkers and a pistol.', 'not relevant for the story',  'not relevant for the story', 'your question is based on a false assumption', 'quit']</t>
   </si>
   <si>
@@ -179,6 +198,9 @@
   </si>
   <si>
     <t>['a man and a woman are walking into a pub. they order the same drink from the bartender. one of them dies and the other one lives. ', 'not relevant', 'quit']</t>
+  </si>
+  <si>
+    <t>['You have to solve a black stories riddle. I tell you a black story and you have to solve it by asking me questions.', 'Lola goes to a friend of hers and receives a pair of shoes because they did not fit her friend. It will mean her death that same evening.', 'What where they doing together?', 'false assumption they', 'ask about the hobbies of the man', 'what could have been different with other shoes', 'Could he see where he was aiming?', 'ik keur hem goed!']</t>
   </si>
 </sst>
 </file>
@@ -546,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +640,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2">
         <v>16</v>
@@ -627,7 +649,7 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -656,7 +678,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3">
         <v>15</v>
@@ -665,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -694,7 +716,7 @@
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4">
         <v>12</v>
@@ -703,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -732,7 +754,7 @@
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -741,7 +763,7 @@
         <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -770,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>8</v>
@@ -779,7 +801,7 @@
         <v>47</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -808,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J7">
         <v>6</v>
@@ -817,7 +839,7 @@
         <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -846,7 +868,7 @@
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J8">
         <v>17</v>
@@ -855,7 +877,7 @@
         <v>32</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -884,7 +906,7 @@
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J9">
         <v>13</v>
@@ -893,7 +915,7 @@
         <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -922,7 +944,7 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J10">
         <v>15</v>
@@ -931,7 +953,7 @@
         <v>39</v>
       </c>
       <c r="L10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -960,7 +982,7 @@
         <v>24</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J11">
         <v>4</v>
@@ -969,7 +991,7 @@
         <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -998,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J12">
         <v>5</v>
@@ -1007,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1036,7 +1058,7 @@
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J13">
         <v>5</v>
@@ -1045,7 +1067,7 @@
         <v>16</v>
       </c>
       <c r="L13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1074,7 +1096,7 @@
         <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J14">
         <v>6</v>
@@ -1083,7 +1105,45 @@
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>66</v>
+      </c>
+      <c r="G15">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update files & excel
</commit_message>
<xml_diff>
--- a/NHC_analysis.xlsx
+++ b/NHC_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linth\PycharmProjects\Scientific_Prog\GitHub\BlackStoriesAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0539E0F-30D9-4B92-9E8E-878C43E85F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2809AA0-AB8E-4010-8E0F-5622943741DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>Medium</t>
   </si>
@@ -122,6 +122,18 @@
     <t>['Linthe Van Rooij: You have to solve a black stories riddle. I tell you a black story and you have to solve it by asking me questions.', 'Linthe Van Rooij: Lola goes to a friend of hers and receives a pair of shoes because they did not fit her friend. It will mean her death that same evening.', 'Thijs : Is her death related to the shoes', 'Linthe Van Rooij: yes', 'Thijs : Are they regular shoes?', 'Linthe Van Rooij: yes', 'Thijs : Is her friend willingly giving the shoes?', 'Linthe Van Rooij: yes', 'Thijs : Does her friend know about the death when it is happening', 'Linthe Van Rooij: no', 'Thijs : Did she die naturally?', 'Linthe Van Rooij: no', 'Thijs : She was murdered?', 'Linthe Van Rooij: no', 'Thijs : Accident?', 'Linthe Van Rooij: yes', 'Thijs : Did she trip because of the shoes?', 'Linthe Van Rooij: no', 'Thijs : Did sure have the shoes on when she died?', 'Linthe Van Rooij: yes', 'Thijs : Was there anything off about the shoes?', 'Linthe Van Rooij: no', 'Thijs : Was there anyone else involved in her death', 'Linthe Van Rooij: yes', 'Thijs : Did that person want the shoes', 'Linthe Van Rooij: no', 'Thijs : Did they make the accident happen', 'Linthe Van Rooij: yes', 'Thijs : Was the accident at home', 'Linthe Van Rooij: yes', 'Thijs : Was it her husband?', 'Linthe Van Rooij: yes', 'Thijs : Was her husband having an affair with the friend', 'Linthe Van Rooij: no', 'Thijs : Did she die because of air restriction? E.g. choked', 'Linthe Van Rooij: no', 'Linthe Van Rooij: What where they doing together?', "Thijs : We're they dancing?", 'Linthe Van Rooij: no', "Thijs : We're they moving", 'Linthe Van Rooij: false assumption they', 'Thijs : Was she moving', 'Linthe Van Rooij: no', 'Thijs : Was he moving', 'Linthe Van Rooij: yes', 'Thijs : Did he kill her by accident', 'Linthe Van Rooij: yes', 'Thijs : Did he trip over the shoes', 'Linthe Van Rooij: no', 'Thijs : Did he stab her', 'Linthe Van Rooij: no', 'Thijs : Was he taking a shower', 'Linthe Van Rooij: no', 'Thijs : Were they eating', 'Linthe Van Rooij: no', 'Thijs : Sleeping?', 'Linthe Van Rooij: no', 'Thijs : Cooking', 'Linthe Van Rooij: no', 'Thijs : Did he scare her', 'Linthe Van Rooij: no', 'Thijs : Hint', 'Linthe Van Rooij: ask about the hobbies of the man', 'Thijs : Was he a shoe maker', 'Linthe Van Rooij: no', 'Thijs : Did he have a workshop', 'Linthe Van Rooij: no', 'Thijs : Anything clothes, food or fashion related hobbies?', 'Linthe Van Rooij: no', 'Thijs : Anything with weapons?', 'Linthe Van Rooij: yes', 'Thijs : Swords?', 'Linthe Van Rooij: no', 'Thijs : Guns', 'Linthe Van Rooij: no', 'Thijs : Bow and arrow', 'Linthe Van Rooij: yes', 'Thijs : Did her shoes look like a target', 'Linthe Van Rooij: no', 'Thijs : Did he shoot her with an arrow', 'Linthe Van Rooij: yes', 'Linthe Van Rooij: what could have been different with other shoes', 'Thijs : Did he think she was an intruder', 'Linthe Van Rooij: no', 'Thijs : Did she have the same shoes as his targets', 'Linthe Van Rooij: no', 'Thijs : Was she taller because of the shoes', 'Linthe Van Rooij: yes', 'Thijs : Did he practice shooting stuff from her head but now she is taller thus he shot her in the head', 'Linthe Van Rooij: no', 'Thijs : Was she taller than a safety wall, so she could get hit', 'Linthe Van Rooij: no', 'Linthe Van Rooij: Could he see where he was aiming?', 'Thijs : Was he blind or blondfolded', 'Linthe Van Rooij: yes', 'Thijs : So he shoots arrows blind, and she hold up a target ðŸŽ¯, but because she is taller he missed and hit her', 'Linthe Van Rooij: ik keur hem goed!']</t>
   </si>
   <si>
+    <t>['Linthe Van Rooij: A woman dies after lighting a lighter, and doesnâ€™t even need a funeral.', 'Thijs : Did she die in a fire or die from the smoke of the fire', 'Linthe Van Rooij: No', 'Thijs : Was she already burried?', 'Linthe Van Rooij: Yes', 'Thijs : Was she already presumed to be dead?', 'Linthe Van Rooij: No', 'Thijs : Did she fall in a coffin?', 'Linthe Van Rooij: No', 'Thijs : But she is in a coffin?', 'Linthe Van Rooij: Yes', 'Thijs : She lit the lighter to see that she was buried?', 'Linthe Van Rooij: No', 'Thijs : Was she mistaken for someone else?', 'Linthe Van Rooij: No', 'Thijs : Was she in the coffin by accident?', 'Linthe Van Rooij: No', 'Thijs : Was she looking for someone in the coffin?', 'Linthe Van Rooij: No', 'Thijs : Did people already think that she was dead?', 'Linthe Van Rooij: No', 'Thijs : Did she fall asleep in the coffin?', 'Linthe Van Rooij: No', 'Thijs : Was there anyone else involved in her death?', 'Linthe Van Rooij: Yes', 'Thijs : Did that person try to kill/murder her or accidentally kill her?', 'Linthe Van Rooij: No', 'Thijs : Was that person alive?', 'Linthe Van Rooij: No', 'Thijs : Did she suffocate?', 'Linthe Van Rooij: Yes', 'Thijs : Did she dig the hole that she was in herself?', 'Linthe Van Rooij: No', 'Thijs : Hint', 'Linthe Van Rooij: Ask about the occupation of the other person involved', 'Thijs : Was the other person a gravedigger or involved at the graveyard?', 'Linthe Van Rooij: Yes', 'Thijs : Was there anyone else involved', 'Linthe Van Rooij: No', 'Thijs : Was the gravedigger digging her grave?', 'Linthe Van Rooij: No', 'Thijs : Was the gravedigger already dead when she met him?', 'Linthe Van Rooij: No', 'Thijs : Did they fight and she killed him?', 'Linthe Van Rooij: No', 'Thijs : Did she know him?', 'Linthe Van Rooij: Yes', 'Thijs : Was she related to him?', 'Linthe Van Rooij: No', 'Thijs : Were they partners', 'Linthe Van Rooij: No', 'Linthe Van Rooij: Why did she lit the lighter inside the coffin?', 'Thijs : To set something on fire or to signal something?', 'Linthe Van Rooij: No', 'Thijs : To light a cigarette or to suffocate herself?', 'Linthe Van Rooij: No', 'Thijs : Was the other person with her inside or the coffin?', 'Linthe Van Rooij: Yes', 'Thijs : Did she light it to kill him or to do anything related to him?', 'Linthe Van Rooij: No', 'Thijs : Did she take a shortcut home through the graveyard?', 'Linthe Van Rooij: No', 'Thijs : Did the guy fall in the coffin?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: Ask about where she was before', 'Thijs : Was she at a funeral?', 'Linthe Van Rooij: No', 'Thijs : At a social event?', 'Linthe Van Rooij: No', 'Thijs : Was she visiting someone at the graveyard or was she running?', 'Linthe Van Rooij: No', 'Thijs : Was she walking', 'Linthe Van Rooij: No', 'Thijs : Was she scared of the gravedigger', 'Linthe Van Rooij: No', 'Thijs : Was she at home', 'Linthe Van Rooij: No', 'Thijs : Anything sport related or food related', 'Linthe Van Rooij: No', 'Thijs : Was she drunk or on drugs', 'Linthe Van Rooij: No', 'Thijs : Was she shopping or in town', 'Linthe Van Rooij: No', 'Thijs : Was it night', 'Linthe Van Rooij: Not relevant', 'Thijs : Was she driving around', 'Linthe Van Rooij: No', 'Thijs : Hint', 'Linthe Van Rooij: She was a criminal/convict', 'Thijs : Did she just rob the house of the gravedigger', 'Linthe Van Rooij: No', 'Thijs : Did she rob someone who died', 'Linthe Van Rooij: No', 'Thijs : Did she just rob someone', 'Linthe Van Rooij: No', 'Thijs : Did she just murder someone?', 'Linthe Van Rooij: No', 'Thijs : Was she escaping prison', 'Linthe Van Rooij: Yes', 'Thijs : And she was hiding in the grave to escape the police?', 'Linthe Van Rooij: Yes', 'Thijs : And the gravedigger was an accomplice?', 'Linthe Van Rooij: Yes', 'Thijs : So they tried to hide from the police by hiding in the grave but they got locked in', 'Linthe Van Rooij: No', 'Thijs : She tried to hide from the police in the grave that the gravedigger made for her, but he was also dead in the coffin so they were trapped, she lit the lighter to confirm that he was dead', 'Linthe Van Rooij: She expected another person to be in the grave next to her', 'Thijs : She tried to escape the prison through the coffin of someone else, and the gravedigger was supposed to get her out, but the coffin was for the gravedigger thus he could not get her out, she used the lighter to see the face of the person that was in the coffin with her', 'Linthe Van Rooij: Allrightyy']</t>
+  </si>
+  <si>
+    <t>['Linthe Van Rooij: A man goes into a cafe and orders a glass of coke. The woman behind the bar grabs a knife and pointed it towards the man. He thanks her and leaves.', 'Lynn van Zeijts: is one of them going to die after she leaves?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: do they have an important conversation after he received the coke?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: does the men also has a weapon?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: will he take the knife of the women?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is she leaving with the knife in her hand?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the men ask the women for a knife?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is one the men or the women getting injured?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: are there more people involved except the men &amp; women?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is it important to know why the women decides to leave?', 'Linthe Van Rooij: Yes', 'Linthe Van Rooij: False assumption woman leaves', 'Lynn van Zeijts: so HE leaves? (not she)', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did the  men pay for his coke?', 'Lynn van Zeijts: is the relation between the men &amp; women important?', 'Linthe Van Rooij: Not relevant', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the women aimed to threaten him with the knife?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the women ask him to do something with the knife because she did not want to do something?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the men insult the women?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the men do something which can be seen considerd as ethically wrong?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: Ask about why he orders something at the bar', 'Lynn van Zeijts: did he order a coke to celebrate something?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did he order something because had some medical emergency?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did he order something for a negative reason?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: was this negative reason related to the women?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: was this related to his work?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: to his family live?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is the fact that he order coke (and not another drink) important to understand the negative event?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did he revelaed a secret?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the men receive his coke before she grabbed the knife?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the men threatend the women as well?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: so did the women refused to give him the coke?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the negative event happended shortly before he entered the cafe?', 'Linthe Van Rooij: No, it is still happening', 'Lynn van Zeijts: did they got into a fight?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the men drink anything before he order the coke?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: The drink could serve as a remedy for the event', 'Lynn van Zeijts: were there any other elements or objects involved, caused the negative event?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is the coke dangerous for him?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is the negative event over once he leaves the cafe?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: is the women trying to help the men by showing the knife?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: does the men wants to kill himself?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: does the women wants to kill or injure him?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: does the women wants to break or open anything related to the men (rope, hair, a bag ect)?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: She only wants to scare him', 'Lynn van Zeijts: to protect herself?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: to protect and help him?', 'Linthe Van Rooij: Ask these questions seperately', 'Lynn van Zeijts: is the women trying to help the men by scaring him with the knife?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: Did the men had a hiccup, and therefore asked for a coke. However, this did not work. Therefore the women tried to scared him with a knife. As a result, the hiccup went away and the men thanked her for her help.', 'Linthe Van Rooij: Yes!!!!!!! You got it']</t>
+  </si>
+  <si>
+    <t>['Linthe Van Rooij: A man climbs out of a large vehicle and drowned himself', 'Lynn van Zeijts: is the vehicle still on land when he climbs out the vehicle?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: is the vehicle close to water as well?', 'Linthe Van Rooij: Not relevant', 'Lynn van Zeijts: were there any other people in the vehicle as well?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: was this vehicle an airplane?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is this vehicle used for public transport?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is it relevant to know the type of vehicle?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: is the vehicle made to be on land?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: is it a tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did he drown himself on purpose?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: was he a farmer?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did something negative happened to his farming practices?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did something negative happened at all?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: does this has anything to do with the tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: was the tractor broken?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: was the land, in which the tractor was located at that moment boggy?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the reason that he climbed out of the tractor had anything to do with the tractor?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: was the water in which he drowned himself close to the tractor?', 'Linthe Van Rooij: Not relevant', 'Lynn van Zeijts: were there any other objects or people involved in the negative event?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: were there any people in the tractor?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: outside the tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did he wanted to go to the other people?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the drowning happened right after he climbed out of the tractor?', 'Linthe Van Rooij: Not relevant', 'Lynn van Zeijts: did the other people influenced him in stepping out of the tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: was it dangerous for him to stay in the vehicle?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: were the other people also with tractors? n', 'Linthe Van Rooij: No', 'Lynn van Zeijts: is it important to know how he exactly climbed out of the tractor?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: Ask about the relationship with the people involved', 'Lynn van Zeijts: did the other people wanted him to drown himself?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the other people wanted to save him?', 'Lynn van Zeijts: did he know the other people before?', 'Linthe Van Rooij: Yes', 'Linthe Van Rooij: Not relevant', 'Lynn van Zeijts: was it an accident that he drowned?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the other people saw something which the men could not see (when he was still in the tractor)?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: were the other people also farmers?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: were the other people angry at him?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: did the know eachother for a long time?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: were they employees?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: family?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: were they close to the tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: was there a fight or any other negative event between the men and his family?', 'Linthe Van Rooij: No', 'Lynn van Zeijts: were there any childern involved?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: were the childeren outside the tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did he climbed out the tractor for his childern?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: was his kid in a dangerous situation?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did he aimed to save his kid by climbing out of the tractor?', 'Lynn van Zeijts: did he cause the dangerous situation?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: did he accidently killed his kid with his tractor?', 'Linthe Van Rooij: Yes', 'Lynn van Zeijts: so he accidently he run over the kid with his tractor because he did not saw him because they were playing the field so he drowned himself somewhere afterwards because it made him so depressed']</t>
+  </si>
+  <si>
+    <t>['Linthe Van Rooij: A man and a woman are seated at a table. On the table between them is a game of checkers and a pistol.', 'PiÃ±a: Did someone die?', 'PiÃ±a: Are they loved ones?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: Not relevant', 'PiÃ±a: Were they playing checkers together?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Can the winner do something with the pistol?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Can the winner kill the loser with the pistol?', 'Linthe Van Rooij: No', 'PiÃ±a: Is someone going to shoot with the pistol?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Did the woman win?', 'Linthe Van Rooij: Not relevant', 'PiÃ±a: Did the man or woman shot another person in the room?', 'Linthe Van Rooij: No', 'PiÃ±a: Were there other people in the room?', 'Linthe Van Rooij: No', 'PiÃ±a: Did someone shoot in the air?', 'Linthe Van Rooij: No', 'PiÃ±a: Did one of the two people kill the other?', 'Linthe Van Rooij: No', 'PiÃ±a: I mean did one shot the other?', 'Linthe Van Rooij: No', 'PiÃ±a: But there was a shot?', 'Linthe Van Rooij: No', 'PiÃ±a: But there was a shot but not on a person?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: there was no shot but there is going to be', 'PiÃ±a: Can the winner use the pistol to make a shot?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Will the winner of the game shoot the other player after winning the game of checkers?', 'Linthe Van Rooij: No', 'PiÃ±a: Will someone die in the future?', 'Linthe Van Rooij: Yes', 'PiÃ±a: One of the two players?', 'Linthe Van Rooij: Yes', 'PiÃ±a: The winner?', 'Linthe Van Rooij: Yes', 'PiÃ±a: The loser is so sad and mad that they shot the winner?', 'Linthe Van Rooij: No', 'PiÃ±a: They are playing the game because someone has to die?', 'Linthe Van Rooij: No', 'PiÃ±a: The winner shot themselves?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Is the why of this question relevant?', 'Linthe Van Rooij: Yes', 'Linthe Van Rooij: Ask about the location', 'PiÃ±a: Were they in jail?', 'Linthe Van Rooij: No', 'PiÃ±a: Were they in a bar?', 'Linthe Van Rooij: No', 'PiÃ±a: Were they in an unusual place to play the game?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Were they outside?', 'Linthe Van Rooij: No', 'PiÃ±a: At someoneâ€™s house?', 'Linthe Van Rooij: No', 'PiÃ±a: Were they going from a place to another place while playing the game?', 'Linthe Van Rooij: No', 'PiÃ±a: This is so hard, can you give me another hint', 'Linthe Van Rooij: They are in some kind of vehicle', 'PiÃ±a: In a plane?', 'Linthe Van Rooij: No', 'PiÃ±a: In a train?', 'Linthe Van Rooij: No', 'PiÃ±a: In a bus?', 'Linthe Van Rooij: No', 'PiÃ±a: In a car?', 'Linthe Van Rooij: No', 'PiÃ±a: In a boat?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Did someone shoot a hole in the boat?', 'Linthe Van Rooij: No', 'Linthe Van Rooij: The type of boat is relevant to the story', 'PiÃ±a: Okay summary, two players are on a boat playing checkers, the winner fires a shot with the pistol in the future on theirselves', 'Linthe Van Rooij: Yes', 'PiÃ±a: Is it a cruise?', 'Linthe Van Rooij: No', 'PiÃ±a: A big boat?', 'Linthe Van Rooij: No', 'PiÃ±a: Or a small boat for just the two of them?', 'Linthe Van Rooij: Yes', 'PiÃ±a: A rowing boat?', 'Linthe Van Rooij: No', 'PiÃ±a: A rubber boat?', 'Linthe Van Rooij: No', 'PiÃ±a: The boat was big enough for a table right?', 'Linthe Van Rooij: Yes', 'PiÃ±a: An expensive boat?', 'Linthe Van Rooij: Yes', 'PiÃ±a: A yacht?', 'Linthe Van Rooij: No', 'PiÃ±a: A sailing boat?', 'Linthe Van Rooij: No', 'PiÃ±a: I just named all boat types haha, do I have to go in a different direction?', 'Linthe Van Rooij: Yes, under water', 'PiÃ±a: A submarine?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Is why they were there relevant?', 'Linthe Van Rooij: No', 'PiÃ±a: What am I missing?', 'Linthe Van Rooij: Why would you want to shoot yourself in a submarine?', 'PiÃ±a: Because the person was getting crazy?', 'Linthe Van Rooij: No', 'PiÃ±a: Was the submarine still able to go up after the shot?', 'Linthe Van Rooij: No', 'PiÃ±a: So the person killed everyone in the submarine by the shot?', 'Linthe Van Rooij: No', 'PiÃ±a: Was the shot on themselves intentional?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Does the why they wanted to shot themselves have to do with the game?', 'Linthe Van Rooij: No', 'PiÃ±a: Did it have something to do with the other person?', 'Linthe Van Rooij: No', 'PiÃ±a: Give me more hints please haha I am done with this game', "Linthe Van Rooij: The game is a result of that the submarine can't go up", 'PiÃ±a: Am I even close? I am so bad at this', 'Linthe Van Rooij: Your almost there!!!', 'PiÃ±a: The person who shot themselves was the driver?', 'Linthe Van Rooij: Not relevant', 'PiÃ±a: They were forever stuck there?', 'Linthe Van Rooij: Yes', 'PiÃ±a: They already knew that they were stuck before playing the game?', 'Linthe Van Rooij: Yes', 'PiÃ±a: There was just one bullet?', 'Linthe Van Rooij: Yes', 'PiÃ±a: Ok I think I know now. The people were stuck in a submarine, and they wanted to kill themselves but there was just one bullet in the pistol, they played a game of checkers and the winner could use the bullet to use it to shoot themselves']</t>
+  </si>
+  <si>
     <t>{1: 'Was there a conflict or argument between the man and the woman?', 2: 'Did one of them use the pistol during their time at the table?', 3: 'Is the pistol relevant to the story?', 4: 'Is the game of checkers relevant to the story?', 5: 'Was the result of the checker game influencing what would happen with the pistol?', 6: 'Did they play checkers for their survival?', 7: 'Did the loser of the checker game have to use the pistol on themselves?', 8: 'Did the winner of the checker game have to use the pistol?', 9: 'Was the pistol a stake in the checker game?', 10: 'So, the story is about a man and a woman who decided to play a game of checkers. The pistol on the table was the stake for the game. The winner would get the pistol, but we don\'t know why they wanted it or what they intended to do with it. No one used the pistol during their time at the table.', 11: 'Was the pistol theirs to begin with? Not relevant for the story.', 12: 'Did the man win the checker game? Not relevant for the story.', 13: 'Did they have a plan to use the pistol after the game?', 14: 'Was the pistol meant to be used on someone else not present at the checker game?', 15: 'Were they playing the game to kill time, with an imminent threat lurking, and that\'s why the pistol was placed on the table between them?', 16: 'Did they intend to use the pistol as protection?', 17: 'Did they intend to use the pistol in a celebratory way, like firing it into the air, after the game?', 18: 'Did the intention to use the pistol depended on whether they won or lost the game of checkers?', 19: 'Did they intend to use the pistol to decide something or someone\'s fate?', 20: 'Did the winner of the checkers game get to decide the fate of a third party using the pistol?', 21: 'Did they intend to scare someone with the pistol after the game?', 22: 'Did the game of checkers help them to decide who should use the pistol?', 23: 'Did they play the game of checkers to decide who would be the one to use the pistol to decide the fate of the other person?', 24: 'Did they play the game of checkers to decide who gets to decide their own fate with the pistol?', 25: 'The story is about a man and a woman who are in a desperate situation. They are seated at a table playing a game of checkers, not due to a conflict or a playful challenge. The pistol on the table is a reminder of their bleak situation. The checkers game is not for mere entertainment; the stake is much higher. The winner of the game earns the right to decide their own fate using the pistol. The outcome of the game will decide who gets to use the pistol to make a significant decision about their own life.', 26: 'Is the situation life-threatening?', 27: 'Are they trapped or held hostage in a place from which they are unable to escape?', 28: 'The story revolves around a man and a woman who are trapped or held hostage in a place from which there\'s no escape. Facing a life-threatening situation, they decide to play a game of checkers, with a daunting stake - a pistol placed on the table. They are not playing out of leisure or conflict, but desperation. The winner of the game gets the right to decide their fate with the pistol. Rather than being at the mercy of their captors, they choose this way to have some control over their own lives.', 29: 'Are they trapped in an uninhabited or desolate location with no hope of rescue?', 30: 'Does the winner of the game intend to use the pistol to end his/her own life, to avoid a possibly worse fate?', 31: 'The story is about a man and woman who found themselves trapped in a desolate location with no hope of rescue. They faced dire circumstances and to avoid a possibly worse fate, they decided to play a game of checkers—the stake, however, was not traditional. A pistol was placed on the table, awaiting the game\'s outcome. Through this game, they seized what little control was left in their desperate situation. The winner won the morbid prize—the chance to use the pistol to end their own life, thus escaping the bleak reality before them.', 32: 'Are they trapped at sea on a vessel with no hope of being found?', 33: 'Are they trapped in a cold, desolate place like the Arctic or Antarctic regions?', 34: 'Are they trapped in a desert with no hope for rescue and no way of getting food or water?', 35: 'Are they trapped in a cave or underground with no way out?', 36: 'Are they stranded in space, like on a spaceship or a space station, with no hope of rescue?', 37: 'Are they trapped in a jungle or forest with no means of communication or ability to navigate their way out?', 38: 'Are they trapped in a post-apocalyptic setting without any survival resources?', 39: 'Are they trapped on a high mountain peak with harsh weather conditions and no possibility of rescue?', 40: 'Are they trapped in a war-torn region and the worse fate they fear is falling into the hands of enemy troops or insurgents?', 41: 'Are they trapped in a sinking ship or submerged submarine with no hope of rescue?', 42: 'Will the worse fate they fear be drowning or suffocating due to lack of oxygen in the sinking ship/submarine?', 43: 'Is the worse fate they\'re trying to avoid that of starvation or dehydration while being trapped in the ship/submarine?', 44: 'Did they choose to play a game of checkers to decide who would use the pistol to avoid the slow and painful death of dehydration?', 45: 'The story is about a man and woman, trapped in a submerged submarine with no chance of rescue, faced the grim reality of eventual dehydration. In an attempt to take control of their fate, they decided to play a game of checkers, with a unique stake: a pistol with a single bullet. The outcome of the game would determine who gets to use the pistol, offering a quick escape from their dire situation. The checkers game, thus, became a means for one of them to choose an immediate end over a slow and painful death.'}</t>
   </si>
   <si>
@@ -164,6 +176,18 @@
     <t>['Is her death related to the shoes', 'Are they regular shoes?', 'Is her friend willingly giving the shoes?', 'Does her friend know about the death when it is happening', 'Did she die naturally?', 'She was murdered?', 'Accident?', 'Did she trip because of the shoes?', 'Did sure have the shoes on when she died?', 'Was there anything off about the shoes?', 'Was there anyone else involved in her death', 'Did that person want the shoes', 'Did they make the accident happen', 'Was the accident at home', 'Was it her husband?', 'Was her husband having an affair with the friend', 'Did she die because of air restriction? E.g. choked', "We're they dancing?", "We're they moving", 'Was she moving', 'Was he moving', 'Did he kill her by accident', 'Did he trip over the shoes', 'Did he stab her', 'Was he taking a shower', 'Were they eating', 'Sleeping?', 'Cooking', 'Did he scare her', 'Hint', 'Was he a shoe maker', 'Did he have a workshop', 'Anything clothes, food or fashion related hobbies?', 'Anything with weapons?', 'Swords?', 'Guns', 'Bow and arrow', 'Did her shoes look like a target', 'Did he shoot her with an arrow', 'Did he think she was an intruder', 'Did she have the same shoes as his targets', 'Was she taller because of the shoes', 'Did he practice shooting stuff from her head but now she is taller thus he shot her in the head', 'Was she taller than a safety wall, so she could get hit', 'Was he blind or blondfolded', 'So he shoots arrows blind, and she hold up a target ðŸŽ¯, but because she is taller he missed and hit her']</t>
   </si>
   <si>
+    <t>['Did she die in a fire or die from the smoke of the fire', 'Was she already burried?', 'Was she already presumed to be dead?', 'Did she fall in a coffin?', 'But she is in a coffin?', 'She lit the lighter to see that she was buried?', 'Was she mistaken for someone else?', 'Was she in the coffin by accident?', 'Was she looking for someone in the coffin?', 'Did people already think that she was dead?', 'Did she fall asleep in the coffin?', 'Was there anyone else involved in her death?', 'Did that person try to kill/murder her or accidentally kill her?', 'Was that person alive?', 'Did she suffocate?', 'Did she dig the hole that she was in herself?', 'Hint', 'Was the other person a gravedigger or involved at the graveyard?', 'Was there anyone else involved', 'Was the gravedigger digging her grave?', 'Was the gravedigger already dead when she met him?', 'Did they fight and she killed him?', 'Did she know him?', 'Was she related to him?', 'Were they partners', 'To set something on fire or to signal something?', 'To light a cigarette or to suffocate herself?', 'Was the other person with her inside or the coffin?', 'Did she light it to kill him or to do anything related to him?', 'Did she take a shortcut home through the graveyard?', 'Did the guy fall in the coffin?', 'Was she at a funeral?', 'At a social event?', 'Was she visiting someone at the graveyard or was she running?', 'Was she walking', 'Was she scared of the gravedigger', 'Was she at home', 'Anything sport related or food related', 'Was she drunk or on drugs', 'Was she shopping or in town', 'Was it night', 'Was she driving around', 'Hint', 'Did she just rob the house of the gravedigger', 'Did she rob someone who died', 'Did she just rob someone', 'Did she just murder someone?', 'Was she escaping prison', 'And she was hiding in the grave to escape the police?', 'And the gravedigger was an accomplice?', 'So they tried to hide from the police by hiding in the grave but they got locked in', 'She tried to hide from the police in the grave that the gravedigger made for her, but he was also dead in the coffin so they were trapped, she lit the lighter to confirm that he was dead', 'She tried to escape the prison through the coffin of someone else, and the gravedigger was supposed to get her out, but the coffin was for the gravedigger thus he could not get her out, she used the lighter to see the face of the person that was in the coffin with her']</t>
+  </si>
+  <si>
+    <t>['is one of them going to die after she leaves?', 'do they have an important conversation after he received the coke?', 'does the men also has a weapon?', 'will he take the knife of the women?', 'is she leaving with the knife in her hand?', 'did the men ask the women for a knife?', 'is one the men or the women getting injured?', 'are there more people involved except the men &amp; women?', 'is it important to know why the women decides to leave?', 'so HE leaves? (not she)', 'did the  men pay for his coke?', 'is the relation between the men &amp; women important?', 'did the women aimed to threaten him with the knife?', 'did the women ask him to do something with the knife because she did not want to do something?', 'did the men insult the women?', 'did the men do something which can be seen considerd as ethically wrong?', 'did he order a coke to celebrate something?', 'did he order something because had some medical emergency?', 'did he order something for a negative reason?', 'was this negative reason related to the women?', 'was this related to his work?', 'to his family live?', 'is the fact that he order coke (and not another drink) important to understand the negative event?', 'did he revelaed a secret?', 'did the men receive his coke before she grabbed the knife?', 'did the men threatend the women as well?', 'so did the women refused to give him the coke?', 'did the negative event happended shortly before he entered the cafe?', 'did they got into a fight?', 'did the men drink anything before he order the coke?', 'were there any other elements or objects involved, caused the negative event?', 'is the coke dangerous for him?', 'is the negative event over once he leaves the cafe?', 'is the women trying to help the men by showing the knife?', 'does the men wants to kill himself?', 'does the women wants to kill or injure him?', 'does the women wants to break or open anything related to the men (rope, hair, a bag ect)?', 'to protect herself?', 'to protect and help him?', 'is the women trying to help the men by scaring him with the knife?', 'Did the men had a hiccup, and therefore asked for a coke. However, this did not work. Therefore the women tried to scared him with a knife. As a result, the hiccup went away and the men thanked her for her help.']</t>
+  </si>
+  <si>
+    <t>['is the vehicle still on land when he climbs out the vehicle?', 'is the vehicle close to water as well?', 'were there any other people in the vehicle as well?', 'was this vehicle an airplane?', 'is this vehicle used for public transport?', 'is it relevant to know the type of vehicle?', 'is the vehicle made to be on land?', 'is it a tractor?', 'did he drown himself on purpose?', 'was he a farmer?', 'did something negative happened to his farming practices?', 'did something negative happened at all?', 'does this has anything to do with the tractor?', 'was the tractor broken?', 'was the land, in which the tractor was located at that moment boggy?', 'did the reason that he climbed out of the tractor had anything to do with the tractor?', 'was the water in which he drowned himself close to the tractor?', 'were there any other objects or people involved in the negative event?', 'were there any people in the tractor?', 'outside the tractor?', 'did he wanted to go to the other people?', 'did the drowning happened right after he climbed out of the tractor?', 'did the other people influenced him in stepping out of the tractor?', 'was it dangerous for him to stay in the vehicle?', 'were the other people also with tractors? n', 'is it important to know how he exactly climbed out of the tractor?', 'did the other people wanted him to drown himself?', 'did the other people wanted to save him?', 'did he know the other people before?', 'was it an accident that he drowned?', 'did the other people saw something which the men could not see (when he was still in the tractor)?', 'were the other people also farmers?', 'were the other people angry at him?', 'did the know eachother for a long time?', 'were they employees?', 'family?', 'were they close to the tractor?', 'was there a fight or any other negative event between the men and his family?', 'were there any childern involved?', 'were the childeren outside the tractor?', 'did he climbed out the tractor for his childern?', 'was his kid in a dangerous situation?', 'did he aimed to save his kid by climbing out of the tractor?', 'did he cause the dangerous situation?', 'did he accidently killed his kid with his tractor?', 'so he accidently he run over the kid with his tractor because he did not saw him because they were playing the field so he drowned himself somewhere afterwards because it made him so depressed']</t>
+  </si>
+  <si>
+    <t>['Did someone die?', 'Are they loved ones?', 'Were they playing checkers together?', 'Can the winner do something with the pistol?', 'Can the winner kill the loser with the pistol?', 'Is someone going to shoot with the pistol?', 'Did the woman win?', 'Did the man or woman shot another person in the room?', 'Were there other people in the room?', 'Did someone shoot in the air?', 'Did one of the two people kill the other?', 'I mean did one shot the other?', 'But there was a shot?', 'But there was a shot but not on a person?', 'Can the winner use the pistol to make a shot?', 'Will the winner of the game shoot the other player after winning the game of checkers?', 'Will someone die in the future?', 'One of the two players?', 'The winner?', 'The loser is so sad and mad that they shot the winner?', 'They are playing the game because someone has to die?', 'The winner shot themselves?', 'Is the why of this question relevant?', 'Were they in jail?', 'Were they in a bar?', 'Were they in an unusual place to play the game?', 'Were they outside?', 'At someoneâ€™s house?', 'Were they going from a place to another place while playing the game?', 'This is so hard, can you give me another hint', 'In a plane?', 'In a train?', 'In a bus?', 'In a car?', 'In a boat?', 'Did someone shoot a hole in the boat?', 'Okay summary, two players are on a boat playing checkers, the winner fires a shot with the pistol in the future on theirselves', 'Is it a cruise?', 'A big boat?', 'Or a small boat for just the two of them?', 'A rowing boat?', 'A rubber boat?', 'The boat was big enough for a table right?', 'An expensive boat?', 'A yacht?', 'A sailing boat?', 'I just named all boat types haha, do I have to go in a different direction?', 'A submarine?', 'Is why they were there relevant?', 'What am I missing?', 'Because the person was getting crazy?', 'Was the submarine still able to go up after the shot?', 'So the person killed everyone in the submarine by the shot?', 'Was the shot on themselves intentional?', 'Does the why they wanted to shot themselves have to do with the game?', 'Did it have something to do with the other person?', 'Give me more hints please haha I am done with this game', 'Am I even close? I am so bad at this', 'The person who shot themselves was the driver?', 'They were forever stuck there?', 'They already knew that they were stuck before playing the game?', 'There was just one bullet?', 'Ok I think I know now. The people were stuck in a submarine, and they wanted to kill themselves but there was just one bullet in the pistol, they played a game of checkers and the winner could use the bullet to use it to shoot themselves']</t>
+  </si>
+  <si>
     <t>['A man and a woman are seated at a table. On the table between them is a game of checkers and a pistol.', 'not relevant for the story',  'not relevant for the story', 'your question is based on a false assumption', 'quit']</t>
   </si>
   <si>
@@ -201,6 +225,18 @@
   </si>
   <si>
     <t>['You have to solve a black stories riddle. I tell you a black story and you have to solve it by asking me questions.', 'Lola goes to a friend of hers and receives a pair of shoes because they did not fit her friend. It will mean her death that same evening.', 'What where they doing together?', 'false assumption they', 'ask about the hobbies of the man', 'what could have been different with other shoes', 'Could he see where he was aiming?', 'ik keur hem goed!']</t>
+  </si>
+  <si>
+    <t>['A woman dies after lighting a lighter, and doesnâ€™t even need a funeral.', 'Ask about the occupation of the other person involved', 'Why did she lit the lighter inside the coffin?', 'Ask about where she was before', 'Not relevant', 'She was a criminal/convict', 'She expected another person to be in the grave next to her', 'Allrightyy']</t>
+  </si>
+  <si>
+    <t>['A man goes into a cafe and orders a glass of coke. The woman behind the bar grabs a knife and pointed it towards the man. He thanks her and leaves.', 'False assumption woman leaves', 'Not relevant', 'Ask about why he orders something at the bar', 'No, it is still happening', 'The drink could serve as a remedy for the event', 'She only wants to scare him', 'Ask these questions seperately', 'Yes!!!!!!! You got it']</t>
+  </si>
+  <si>
+    <t>['A man climbs out of a large vehicle and drowned himself', 'Not relevant', 'Not relevant', 'Not relevant', 'Ask about the relationship with the people involved', 'Not relevant']</t>
+  </si>
+  <si>
+    <t>['A man and a woman are seated at a table. On the table between them is a game of checkers and a pistol.', 'Not relevant', 'Not relevant', 'there was no shot but there is going to be', 'Ask about the location', 'They are in some kind of vehicle', 'The type of boat is relevant to the story', 'Yes, under water', 'Why would you want to shoot yourself in a submarine?', "The game is a result of that the submarine can't go up", 'Your almost there!!!', 'Not relevant']</t>
   </si>
 </sst>
 </file>
@@ -568,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J2">
         <v>16</v>
@@ -649,7 +685,7 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -678,7 +714,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J3">
         <v>15</v>
@@ -687,7 +723,7 @@
         <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -716,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J4">
         <v>12</v>
@@ -725,7 +761,7 @@
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -754,7 +790,7 @@
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -763,7 +799,7 @@
         <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -792,7 +828,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J6">
         <v>8</v>
@@ -801,7 +837,7 @@
         <v>47</v>
       </c>
       <c r="L6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -830,7 +866,7 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J7">
         <v>6</v>
@@ -839,7 +875,7 @@
         <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -868,7 +904,7 @@
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J8">
         <v>17</v>
@@ -877,7 +913,7 @@
         <v>32</v>
       </c>
       <c r="L8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -906,7 +942,7 @@
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J9">
         <v>13</v>
@@ -915,7 +951,7 @@
         <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -944,7 +980,7 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J10">
         <v>15</v>
@@ -953,7 +989,7 @@
         <v>39</v>
       </c>
       <c r="L10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -982,7 +1018,7 @@
         <v>24</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J11">
         <v>4</v>
@@ -991,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1020,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J12">
         <v>5</v>
@@ -1029,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1058,7 +1094,7 @@
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J13">
         <v>5</v>
@@ -1067,7 +1103,7 @@
         <v>16</v>
       </c>
       <c r="L13" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1096,7 +1132,7 @@
         <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J14">
         <v>6</v>
@@ -1105,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1134,7 +1170,7 @@
         <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J15">
         <v>16</v>
@@ -1143,10 +1179,163 @@
         <v>28</v>
       </c>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>78</v>
+      </c>
+      <c r="G16">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <v>40</v>
+      </c>
+      <c r="L16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>41</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>61</v>
+      </c>
+      <c r="G17">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+      <c r="K17">
+        <v>33</v>
+      </c>
+      <c r="L17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>46</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>51</v>
+      </c>
+      <c r="G18">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18">
+        <v>22</v>
+      </c>
+      <c r="K18">
+        <v>23</v>
+      </c>
+      <c r="L18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>63</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>98</v>
+      </c>
+      <c r="G19">
+        <v>24</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <v>21</v>
+      </c>
+      <c r="K19">
+        <v>38</v>
+      </c>
+      <c r="L19" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>